<commit_message>
Changes Done in All field
</commit_message>
<xml_diff>
--- a/asset.xlsx
+++ b/asset.xlsx
@@ -397,7 +397,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:N275"/>
+  <dimension ref="A1:N278"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -3147,7 +3147,7 @@
         <v>LAP-000062</v>
       </c>
       <c r="F63" t="str">
-        <v>In Use</v>
+        <v>Spare</v>
       </c>
       <c r="G63" t="str">
         <v>ILOG</v>
@@ -4731,7 +4731,7 @@
         <v>LAP-000098</v>
       </c>
       <c r="F99" t="str">
-        <v>In Use</v>
+        <v>Spare</v>
       </c>
       <c r="G99" t="str">
         <v>ILOG</v>
@@ -7591,7 +7591,7 @@
         <v>MOB-000001</v>
       </c>
       <c r="F164" t="str">
-        <v>In Use</v>
+        <v>Spare</v>
       </c>
       <c r="G164" t="str">
         <v>ilog</v>
@@ -8984,19 +8984,19 @@
     </row>
     <row r="196">
       <c r="A196" t="str">
-        <v>Laptop</v>
+        <v>Desktop</v>
       </c>
       <c r="B196" t="str">
         <v>Lenovo</v>
       </c>
       <c r="C196" t="str">
-        <v>X1 Yoga</v>
+        <v>LENOVO 599</v>
       </c>
       <c r="D196" t="str">
-        <v>R90MZVX7</v>
+        <v>L9HK853</v>
       </c>
       <c r="E196" t="str">
-        <v>LAP-000002</v>
+        <v>DES-000036</v>
       </c>
       <c r="F196" t="str">
         <v>In Use</v>
@@ -9005,42 +9005,42 @@
         <v>ILOG</v>
       </c>
       <c r="H196" t="str">
-        <v>2022-04-01</v>
+        <v>2023-06-08</v>
       </c>
       <c r="I196" t="str">
-        <v>MM Computer Communication</v>
+        <v>MISC VENDOR</v>
       </c>
       <c r="J196" t="str">
-        <v>Rental</v>
+        <v>Owned</v>
       </c>
       <c r="K196" t="str">
-        <v>HO</v>
+        <v>LKO-AWL</v>
       </c>
       <c r="L196" t="str">
-        <v>RENT4-HO-RRP</v>
+        <v>LKO FIREWALL 9.3.3</v>
       </c>
       <c r="M196" t="str">
-        <v>Rituraj Pankaj</v>
+        <v>IT SUPPORT</v>
       </c>
       <c r="N196" t="str">
-        <v>RIT8868</v>
+        <v>IT 6771</v>
       </c>
     </row>
     <row r="197">
       <c r="A197" t="str">
-        <v>Data Card</v>
+        <v>Laptop</v>
       </c>
       <c r="B197" t="str">
-        <v>Airtel</v>
+        <v>HP</v>
       </c>
       <c r="C197" t="str">
-        <v>MW40CJ-BATIN3</v>
+        <v>HP 440 G5</v>
       </c>
       <c r="D197" t="str">
-        <v>7042228703</v>
+        <v>5CD8135YDV</v>
       </c>
       <c r="E197" t="str">
-        <v>DAT-000001</v>
+        <v>LAP-000134</v>
       </c>
       <c r="F197" t="str">
         <v>In Use</v>
@@ -9049,25 +9049,25 @@
         <v>ILOG</v>
       </c>
       <c r="H197" t="str">
-        <v>2022-04-01</v>
+        <v>2023-06-08</v>
       </c>
       <c r="I197" t="str">
-        <v>AIRTEL</v>
+        <v>Onsite Computer Solutions</v>
       </c>
       <c r="J197" t="str">
         <v>Rental</v>
       </c>
       <c r="K197" t="str">
-        <v>HO</v>
+        <v>GGN2-AWL</v>
       </c>
       <c r="L197" t="str">
-        <v>Data Card - 7042228703</v>
+        <v>RENT8-GGN2-DEVENDER</v>
       </c>
       <c r="M197" t="str">
-        <v>Rituraj Pankaj</v>
+        <v>Devender Kumar</v>
       </c>
       <c r="N197" t="str">
-        <v>RIT8868</v>
+        <v>DEV5502</v>
       </c>
     </row>
     <row r="198">
@@ -9078,22 +9078,22 @@
         <v>Airtel</v>
       </c>
       <c r="C198" t="str">
-        <v>Airtel Smart</v>
+        <v>SIM CARD</v>
       </c>
       <c r="D198" t="str">
-        <v>9205390764</v>
+        <v>9205390743</v>
       </c>
       <c r="E198" t="str">
-        <v>SIM-000001</v>
+        <v>SIM-000003</v>
       </c>
       <c r="F198" t="str">
-        <v>In Use</v>
+        <v>Spare</v>
       </c>
       <c r="G198" t="str">
-        <v>AWL</v>
+        <v>ILOG</v>
       </c>
       <c r="H198" t="str">
-        <v>2022-10-01</v>
+        <v>2023-06-09</v>
       </c>
       <c r="I198" t="str">
         <v>AIRTEL</v>
@@ -9105,74 +9105,74 @@
         <v>HO</v>
       </c>
       <c r="L198" t="str">
-        <v>SIM - 9205390764</v>
+        <v>SIM CARD</v>
       </c>
       <c r="M198" t="str">
-        <v>Yuvraj Singh</v>
+        <v>Jahanvi Singh</v>
       </c>
       <c r="N198" t="str">
-        <v>YUV1621</v>
+        <v>JAH7056</v>
       </c>
     </row>
     <row r="199">
       <c r="A199" t="str">
-        <v>SIM (only)</v>
+        <v>Laptop</v>
       </c>
       <c r="B199" t="str">
-        <v>Airtel</v>
+        <v>Lenovo</v>
       </c>
       <c r="C199" t="str">
-        <v>Airtel Smart</v>
+        <v>X1 Yoga</v>
       </c>
       <c r="D199" t="str">
-        <v>7043144456</v>
+        <v>R90MZVX7</v>
       </c>
       <c r="E199" t="str">
-        <v>SIM-000002</v>
+        <v>LAP-000002</v>
       </c>
       <c r="F199" t="str">
         <v>In Use</v>
       </c>
       <c r="G199" t="str">
-        <v>AWL</v>
+        <v>ILOG</v>
       </c>
       <c r="H199" t="str">
-        <v>2020-08-21</v>
+        <v>2022-04-01</v>
       </c>
       <c r="I199" t="str">
-        <v>AIRTEL</v>
+        <v>MM Computer Communication</v>
       </c>
       <c r="J199" t="str">
         <v>Rental</v>
       </c>
       <c r="K199" t="str">
-        <v>AHM-AWL</v>
+        <v>HO</v>
       </c>
       <c r="L199" t="str">
-        <v>SIM - 7043144456</v>
+        <v>RENT4-HO-RRP</v>
       </c>
       <c r="M199" t="str">
-        <v>Vikas Pandya</v>
+        <v>Rituraj Pankaj</v>
       </c>
       <c r="N199" t="str">
-        <v>VIK9088</v>
+        <v>RIT8868</v>
       </c>
     </row>
     <row r="200">
       <c r="A200" t="str">
-        <v>Laptop</v>
+        <v>Data Card</v>
       </c>
       <c r="B200" t="str">
-        <v>HP</v>
+        <v>Airtel</v>
       </c>
       <c r="C200" t="str">
-        <v>Elitebook 840 G1</v>
+        <v>MW40CJ-BATIN3</v>
       </c>
       <c r="D200" t="str">
-        <v>5CG447487B</v>
+        <v>7042228703</v>
       </c>
       <c r="E200" t="str">
-        <v>LAP-000003</v>
+        <v>DAT-000001</v>
       </c>
       <c r="F200" t="str">
         <v>In Use</v>
@@ -9181,42 +9181,42 @@
         <v>ILOG</v>
       </c>
       <c r="H200" t="str">
-        <v>2020-04-01</v>
+        <v>2022-04-01</v>
       </c>
       <c r="I200" t="str">
-        <v>MM Computer Communication</v>
+        <v>AIRTEL</v>
       </c>
       <c r="J200" t="str">
         <v>Rental</v>
       </c>
       <c r="K200" t="str">
-        <v>AHM-AWL</v>
+        <v>HO</v>
       </c>
       <c r="L200" t="str">
-        <v>RENT4-AHD-VPANDYA</v>
+        <v>Data Card - 7042228703</v>
       </c>
       <c r="M200" t="str">
-        <v>Vikas Pandya</v>
+        <v>Rituraj Pankaj</v>
       </c>
       <c r="N200" t="str">
-        <v>VIK9088</v>
+        <v>RIT8868</v>
       </c>
     </row>
     <row r="201">
       <c r="A201" t="str">
-        <v>Digital Camera</v>
+        <v>SIM (only)</v>
       </c>
       <c r="B201" t="str">
-        <v>Canon</v>
+        <v>Airtel</v>
       </c>
       <c r="C201" t="str">
-        <v>Powershot A800</v>
+        <v>Airtel Smart</v>
       </c>
       <c r="D201" t="str">
-        <v>228063335362</v>
+        <v>9205390764</v>
       </c>
       <c r="E201" t="str">
-        <v>DIG-000001</v>
+        <v>SIM-000001</v>
       </c>
       <c r="F201" t="str">
         <v>In Use</v>
@@ -9225,54 +9225,54 @@
         <v>AWL</v>
       </c>
       <c r="H201" t="str">
-        <v>2012-12-31</v>
+        <v>2022-10-01</v>
       </c>
       <c r="I201" t="str">
-        <v>MISC VENDOR</v>
+        <v>AIRTEL</v>
       </c>
       <c r="J201" t="str">
-        <v>Owned</v>
+        <v>Rental</v>
       </c>
       <c r="K201" t="str">
-        <v>AHM-AWL</v>
+        <v>HO</v>
       </c>
       <c r="L201" t="str">
-        <v>Canon Powershot A800</v>
+        <v>SIM - 9205390764</v>
       </c>
       <c r="M201" t="str">
-        <v>Vikas Pandya</v>
+        <v>Yuvraj Singh</v>
       </c>
       <c r="N201" t="str">
-        <v>VIK9088</v>
+        <v>YUV1621</v>
       </c>
     </row>
     <row r="202">
       <c r="A202" t="str">
-        <v>Desktop</v>
+        <v>SIM (only)</v>
       </c>
       <c r="B202" t="str">
-        <v>Intel</v>
+        <v>Airtel</v>
       </c>
       <c r="C202" t="str">
-        <v>DH55TC</v>
+        <v>Airtel Smart</v>
       </c>
       <c r="D202" t="str">
-        <v>CDP-DTP-002</v>
+        <v>7043144456</v>
       </c>
       <c r="E202" t="str">
-        <v>DES-000001</v>
+        <v>SIM-000002</v>
       </c>
       <c r="F202" t="str">
         <v>In Use</v>
       </c>
       <c r="G202" t="str">
-        <v>ILOG</v>
+        <v>AWL</v>
       </c>
       <c r="H202" t="str">
-        <v>2020-11-23</v>
+        <v>2020-08-21</v>
       </c>
       <c r="I202" t="str">
-        <v>AAA Rental LLP</v>
+        <v>AIRTEL</v>
       </c>
       <c r="J202" t="str">
         <v>Rental</v>
@@ -9281,7 +9281,7 @@
         <v>AHM-AWL</v>
       </c>
       <c r="L202" t="str">
-        <v>CDP Intel Desktop</v>
+        <v>SIM - 7043144456</v>
       </c>
       <c r="M202" t="str">
         <v>Vikas Pandya</v>
@@ -9292,19 +9292,19 @@
     </row>
     <row r="203">
       <c r="A203" t="str">
-        <v>Data Card</v>
+        <v>Laptop</v>
       </c>
       <c r="B203" t="str">
-        <v>Huawei</v>
+        <v>HP</v>
       </c>
       <c r="C203" t="str">
-        <v>E3372H-607</v>
+        <v>Elitebook 840 G1</v>
       </c>
       <c r="D203" t="str">
-        <v>7042421607</v>
+        <v>5CG447487B</v>
       </c>
       <c r="E203" t="str">
-        <v>DAT-000002</v>
+        <v>LAP-000003</v>
       </c>
       <c r="F203" t="str">
         <v>In Use</v>
@@ -9316,7 +9316,7 @@
         <v>2020-04-01</v>
       </c>
       <c r="I203" t="str">
-        <v>AIRTEL</v>
+        <v>MM Computer Communication</v>
       </c>
       <c r="J203" t="str">
         <v>Rental</v>
@@ -9325,7 +9325,7 @@
         <v>AHM-AWL</v>
       </c>
       <c r="L203" t="str">
-        <v>Data Card - 7042421607</v>
+        <v>RENT4-AHD-VPANDYA</v>
       </c>
       <c r="M203" t="str">
         <v>Vikas Pandya</v>
@@ -9336,19 +9336,19 @@
     </row>
     <row r="204">
       <c r="A204" t="str">
-        <v>Laptop</v>
+        <v>Digital Camera</v>
       </c>
       <c r="B204" t="str">
-        <v>Lenovo</v>
+        <v>Canon</v>
       </c>
       <c r="C204" t="str">
-        <v>B40-80</v>
+        <v>Powershot A800</v>
       </c>
       <c r="D204" t="str">
-        <v>MP10PLH4</v>
+        <v>228063335362</v>
       </c>
       <c r="E204" t="str">
-        <v>LAP-000004</v>
+        <v>DIG-000001</v>
       </c>
       <c r="F204" t="str">
         <v>In Use</v>
@@ -9357,10 +9357,10 @@
         <v>AWL</v>
       </c>
       <c r="H204" t="str">
-        <v>2016-03-02</v>
+        <v>2012-12-31</v>
       </c>
       <c r="I204" t="str">
-        <v>Transtek Infoways Private Limited</v>
+        <v>MISC VENDOR</v>
       </c>
       <c r="J204" t="str">
         <v>Owned</v>
@@ -9369,30 +9369,30 @@
         <v>AHM-AWL</v>
       </c>
       <c r="L204" t="str">
-        <v>AHD-WH-HIREN</v>
+        <v>Canon Powershot A800</v>
       </c>
       <c r="M204" t="str">
-        <v>Parmar Hiren Kumar</v>
+        <v>Vikas Pandya</v>
       </c>
       <c r="N204" t="str">
-        <v>PAR7569</v>
+        <v>VIK9088</v>
       </c>
     </row>
     <row r="205">
       <c r="A205" t="str">
-        <v>Accessories</v>
+        <v>Desktop</v>
       </c>
       <c r="B205" t="str">
-        <v>Comrack</v>
+        <v>Intel</v>
       </c>
       <c r="C205" t="str">
-        <v>Network Rack 6U</v>
+        <v>DH55TC</v>
       </c>
       <c r="D205" t="str">
-        <v>COMRACKGTK1001</v>
+        <v>CDP-DTP-002</v>
       </c>
       <c r="E205" t="str">
-        <v>ACC-000001</v>
+        <v>DES-000001</v>
       </c>
       <c r="F205" t="str">
         <v>In Use</v>
@@ -9401,42 +9401,42 @@
         <v>ILOG</v>
       </c>
       <c r="H205" t="str">
-        <v>2022-06-08</v>
+        <v>2020-11-23</v>
       </c>
       <c r="I205" t="str">
-        <v>MISC VENDOR</v>
+        <v>AAA Rental LLP</v>
       </c>
       <c r="J205" t="str">
-        <v>Owned</v>
+        <v>Rental</v>
       </c>
       <c r="K205" t="str">
-        <v>DEL-AWL</v>
+        <v>AHM-AWL</v>
       </c>
       <c r="L205" t="str">
-        <v>NETWORKING RACK 6U</v>
+        <v>CDP Intel Desktop</v>
       </c>
       <c r="M205" t="str">
-        <v>IT SUPPORT</v>
+        <v>Vikas Pandya</v>
       </c>
       <c r="N205" t="str">
-        <v>IT 6771</v>
+        <v>VIK9088</v>
       </c>
     </row>
     <row r="206">
       <c r="A206" t="str">
-        <v>Accessories</v>
+        <v>Data Card</v>
       </c>
       <c r="B206" t="str">
-        <v>Comrack</v>
+        <v>Huawei</v>
       </c>
       <c r="C206" t="str">
-        <v>Comrack</v>
+        <v>E3372H-607</v>
       </c>
       <c r="D206" t="str">
-        <v>CRKHO001</v>
+        <v>7042421607</v>
       </c>
       <c r="E206" t="str">
-        <v>ACC-000002</v>
+        <v>DAT-000002</v>
       </c>
       <c r="F206" t="str">
         <v>In Use</v>
@@ -9445,69 +9445,69 @@
         <v>ILOG</v>
       </c>
       <c r="H206" t="str">
-        <v>2018-11-23</v>
+        <v>2020-04-01</v>
       </c>
       <c r="I206" t="str">
-        <v>Cybernetic Genesis Private Limited</v>
+        <v>AIRTEL</v>
       </c>
       <c r="J206" t="str">
-        <v>Owned</v>
+        <v>Rental</v>
       </c>
       <c r="K206" t="str">
-        <v>HO</v>
+        <v>AHM-AWL</v>
       </c>
       <c r="L206" t="str">
-        <v>SERVER RACK 42U</v>
+        <v>Data Card - 7042421607</v>
       </c>
       <c r="M206" t="str">
-        <v>IT SUPPORT</v>
+        <v>Vikas Pandya</v>
       </c>
       <c r="N206" t="str">
-        <v>IT 6771</v>
+        <v>VIK9088</v>
       </c>
     </row>
     <row r="207">
       <c r="A207" t="str">
-        <v>Accessories</v>
+        <v>Laptop</v>
       </c>
       <c r="B207" t="str">
-        <v>Comrack</v>
+        <v>Lenovo</v>
       </c>
       <c r="C207" t="str">
-        <v>Comrack</v>
+        <v>B40-80</v>
       </c>
       <c r="D207" t="str">
-        <v>CRKHO002</v>
+        <v>MP10PLH4</v>
       </c>
       <c r="E207" t="str">
-        <v>ACC-000003</v>
+        <v>LAP-000004</v>
       </c>
       <c r="F207" t="str">
         <v>In Use</v>
       </c>
       <c r="G207" t="str">
-        <v>ILOG</v>
+        <v>AWL</v>
       </c>
       <c r="H207" t="str">
-        <v>2018-11-23</v>
+        <v>2016-03-02</v>
       </c>
       <c r="I207" t="str">
-        <v>Cybernetic Genesis Private Limited</v>
+        <v>Transtek Infoways Private Limited</v>
       </c>
       <c r="J207" t="str">
         <v>Owned</v>
       </c>
       <c r="K207" t="str">
-        <v>HO</v>
+        <v>AHM-AWL</v>
       </c>
       <c r="L207" t="str">
-        <v>SERVER RACK 42U</v>
+        <v>AHD-WH-HIREN</v>
       </c>
       <c r="M207" t="str">
-        <v>IT SUPPORT</v>
+        <v>Parmar Hiren Kumar</v>
       </c>
       <c r="N207" t="str">
-        <v>IT 6771</v>
+        <v>PAR7569</v>
       </c>
     </row>
     <row r="208">
@@ -9518,13 +9518,13 @@
         <v>Comrack</v>
       </c>
       <c r="C208" t="str">
-        <v>Comrack</v>
+        <v>Network Rack 6U</v>
       </c>
       <c r="D208" t="str">
-        <v>RACKGGN1001</v>
+        <v>COMRACKGTK1001</v>
       </c>
       <c r="E208" t="str">
-        <v>ACC-000016</v>
+        <v>ACC-000001</v>
       </c>
       <c r="F208" t="str">
         <v>In Use</v>
@@ -9533,7 +9533,7 @@
         <v>ILOG</v>
       </c>
       <c r="H208" t="str">
-        <v>2022-06-07</v>
+        <v>2022-06-08</v>
       </c>
       <c r="I208" t="str">
         <v>MISC VENDOR</v>
@@ -9542,10 +9542,10 @@
         <v>Owned</v>
       </c>
       <c r="K208" t="str">
-        <v>HO</v>
+        <v>DEL-AWL</v>
       </c>
       <c r="L208" t="str">
-        <v>RACK 9U</v>
+        <v>NETWORKING RACK 6U</v>
       </c>
       <c r="M208" t="str">
         <v>IT SUPPORT</v>
@@ -9565,10 +9565,10 @@
         <v>Comrack</v>
       </c>
       <c r="D209" t="str">
-        <v>VRKHO003</v>
+        <v>CRKHO001</v>
       </c>
       <c r="E209" t="str">
-        <v>ACC-000004</v>
+        <v>ACC-000002</v>
       </c>
       <c r="F209" t="str">
         <v>In Use</v>
@@ -9589,7 +9589,7 @@
         <v>HO</v>
       </c>
       <c r="L209" t="str">
-        <v>SERVER RACK 45U</v>
+        <v>SERVER RACK 42U</v>
       </c>
       <c r="M209" t="str">
         <v>IT SUPPORT</v>
@@ -9603,16 +9603,16 @@
         <v>Accessories</v>
       </c>
       <c r="B210" t="str">
-        <v>Matrix</v>
+        <v>Comrack</v>
       </c>
       <c r="C210" t="str">
-        <v>Matrix</v>
+        <v>Comrack</v>
       </c>
       <c r="D210" t="str">
-        <v>EMLOCK001</v>
+        <v>CRKHO002</v>
       </c>
       <c r="E210" t="str">
-        <v>ACC-000005</v>
+        <v>ACC-000003</v>
       </c>
       <c r="F210" t="str">
         <v>In Use</v>
@@ -9621,7 +9621,7 @@
         <v>ILOG</v>
       </c>
       <c r="H210" t="str">
-        <v>2018-12-19</v>
+        <v>2018-11-23</v>
       </c>
       <c r="I210" t="str">
         <v>Cybernetic Genesis Private Limited</v>
@@ -9633,7 +9633,7 @@
         <v>HO</v>
       </c>
       <c r="L210" t="str">
-        <v>ELECTRO MAGNETIC LOCK</v>
+        <v>SERVER RACK 42U</v>
       </c>
       <c r="M210" t="str">
         <v>IT SUPPORT</v>
@@ -9647,16 +9647,16 @@
         <v>Accessories</v>
       </c>
       <c r="B211" t="str">
-        <v>Matrix</v>
+        <v>Comrack</v>
       </c>
       <c r="C211" t="str">
-        <v>Matrix</v>
+        <v>Comrack</v>
       </c>
       <c r="D211" t="str">
-        <v>EMLOCK002</v>
+        <v>RACKGGN1001</v>
       </c>
       <c r="E211" t="str">
-        <v>ACC-000006</v>
+        <v>ACC-000016</v>
       </c>
       <c r="F211" t="str">
         <v>In Use</v>
@@ -9665,10 +9665,10 @@
         <v>ILOG</v>
       </c>
       <c r="H211" t="str">
-        <v>2018-12-19</v>
+        <v>2022-06-07</v>
       </c>
       <c r="I211" t="str">
-        <v>Cybernetic Genesis Private Limited</v>
+        <v>MISC VENDOR</v>
       </c>
       <c r="J211" t="str">
         <v>Owned</v>
@@ -9677,7 +9677,7 @@
         <v>HO</v>
       </c>
       <c r="L211" t="str">
-        <v>ELECTRO MAGNETIC LOCK</v>
+        <v>RACK 9U</v>
       </c>
       <c r="M211" t="str">
         <v>IT SUPPORT</v>
@@ -9691,16 +9691,16 @@
         <v>Accessories</v>
       </c>
       <c r="B212" t="str">
-        <v>Matrix</v>
+        <v>Comrack</v>
       </c>
       <c r="C212" t="str">
-        <v>Matrix</v>
+        <v>Comrack</v>
       </c>
       <c r="D212" t="str">
-        <v>EMLOCK003</v>
+        <v>VRKHO003</v>
       </c>
       <c r="E212" t="str">
-        <v>ACC-000007</v>
+        <v>ACC-000004</v>
       </c>
       <c r="F212" t="str">
         <v>In Use</v>
@@ -9709,7 +9709,7 @@
         <v>ILOG</v>
       </c>
       <c r="H212" t="str">
-        <v>2018-12-19</v>
+        <v>2018-11-23</v>
       </c>
       <c r="I212" t="str">
         <v>Cybernetic Genesis Private Limited</v>
@@ -9721,7 +9721,7 @@
         <v>HO</v>
       </c>
       <c r="L212" t="str">
-        <v>ELECTRO MAGNETIC LOCK</v>
+        <v>SERVER RACK 45U</v>
       </c>
       <c r="M212" t="str">
         <v>IT SUPPORT</v>
@@ -9741,10 +9741,10 @@
         <v>Matrix</v>
       </c>
       <c r="D213" t="str">
-        <v>EMLOCK004</v>
+        <v>EMLOCK001</v>
       </c>
       <c r="E213" t="str">
-        <v>ACC-000008</v>
+        <v>ACC-000005</v>
       </c>
       <c r="F213" t="str">
         <v>In Use</v>
@@ -9785,10 +9785,10 @@
         <v>Matrix</v>
       </c>
       <c r="D214" t="str">
-        <v>EXSWTCH01</v>
+        <v>EMLOCK002</v>
       </c>
       <c r="E214" t="str">
-        <v>ACC-000009</v>
+        <v>ACC-000006</v>
       </c>
       <c r="F214" t="str">
         <v>In Use</v>
@@ -9809,7 +9809,7 @@
         <v>HO</v>
       </c>
       <c r="L214" t="str">
-        <v>EXIT SWITCH</v>
+        <v>ELECTRO MAGNETIC LOCK</v>
       </c>
       <c r="M214" t="str">
         <v>IT SUPPORT</v>
@@ -9829,10 +9829,10 @@
         <v>Matrix</v>
       </c>
       <c r="D215" t="str">
-        <v>EXSWTCH02</v>
+        <v>EMLOCK003</v>
       </c>
       <c r="E215" t="str">
-        <v>ACC-000010</v>
+        <v>ACC-000007</v>
       </c>
       <c r="F215" t="str">
         <v>In Use</v>
@@ -9853,7 +9853,7 @@
         <v>HO</v>
       </c>
       <c r="L215" t="str">
-        <v>EXIT SWITCH</v>
+        <v>ELECTRO MAGNETIC LOCK</v>
       </c>
       <c r="M215" t="str">
         <v>IT SUPPORT</v>
@@ -9867,16 +9867,16 @@
         <v>Accessories</v>
       </c>
       <c r="B216" t="str">
-        <v>Generic</v>
+        <v>Matrix</v>
       </c>
       <c r="C216" t="str">
-        <v>PMKIT001</v>
+        <v>Matrix</v>
       </c>
       <c r="D216" t="str">
-        <v>PMKIT001</v>
+        <v>EMLOCK004</v>
       </c>
       <c r="E216" t="str">
-        <v>ACC-000011</v>
+        <v>ACC-000008</v>
       </c>
       <c r="F216" t="str">
         <v>In Use</v>
@@ -9885,7 +9885,7 @@
         <v>ILOG</v>
       </c>
       <c r="H216" t="str">
-        <v>2018-11-28</v>
+        <v>2018-12-19</v>
       </c>
       <c r="I216" t="str">
         <v>Cybernetic Genesis Private Limited</v>
@@ -9897,7 +9897,7 @@
         <v>HO</v>
       </c>
       <c r="L216" t="str">
-        <v>PROJECTOR MOUNT KIT</v>
+        <v>ELECTRO MAGNETIC LOCK</v>
       </c>
       <c r="M216" t="str">
         <v>IT SUPPORT</v>
@@ -9911,16 +9911,16 @@
         <v>Accessories</v>
       </c>
       <c r="B217" t="str">
-        <v>Generic</v>
+        <v>Matrix</v>
       </c>
       <c r="C217" t="str">
-        <v>PMKIT002</v>
+        <v>Matrix</v>
       </c>
       <c r="D217" t="str">
-        <v>PMKIT002</v>
+        <v>EXSWTCH01</v>
       </c>
       <c r="E217" t="str">
-        <v>ACC-000012</v>
+        <v>ACC-000009</v>
       </c>
       <c r="F217" t="str">
         <v>In Use</v>
@@ -9929,7 +9929,7 @@
         <v>ILOG</v>
       </c>
       <c r="H217" t="str">
-        <v>2018-11-28</v>
+        <v>2018-12-19</v>
       </c>
       <c r="I217" t="str">
         <v>Cybernetic Genesis Private Limited</v>
@@ -9941,7 +9941,7 @@
         <v>HO</v>
       </c>
       <c r="L217" t="str">
-        <v>PROJECTOR MOUNT KIT</v>
+        <v>EXIT SWITCH</v>
       </c>
       <c r="M217" t="str">
         <v>IT SUPPORT</v>
@@ -9955,16 +9955,16 @@
         <v>Accessories</v>
       </c>
       <c r="B218" t="str">
-        <v>Generic</v>
+        <v>Matrix</v>
       </c>
       <c r="C218" t="str">
-        <v>PSCR001</v>
+        <v>Matrix</v>
       </c>
       <c r="D218" t="str">
-        <v>PSCR001</v>
+        <v>EXSWTCH02</v>
       </c>
       <c r="E218" t="str">
-        <v>ACC-000013</v>
+        <v>ACC-000010</v>
       </c>
       <c r="F218" t="str">
         <v>In Use</v>
@@ -9973,7 +9973,7 @@
         <v>ILOG</v>
       </c>
       <c r="H218" t="str">
-        <v>2018-11-28</v>
+        <v>2018-12-19</v>
       </c>
       <c r="I218" t="str">
         <v>Cybernetic Genesis Private Limited</v>
@@ -9985,7 +9985,7 @@
         <v>HO</v>
       </c>
       <c r="L218" t="str">
-        <v>PROJECTION SCREEN</v>
+        <v>EXIT SWITCH</v>
       </c>
       <c r="M218" t="str">
         <v>IT SUPPORT</v>
@@ -10002,13 +10002,13 @@
         <v>Generic</v>
       </c>
       <c r="C219" t="str">
-        <v>PSCR002</v>
+        <v>PMKIT001</v>
       </c>
       <c r="D219" t="str">
-        <v>PSCR002</v>
+        <v>PMKIT001</v>
       </c>
       <c r="E219" t="str">
-        <v>ACC-000014</v>
+        <v>ACC-000011</v>
       </c>
       <c r="F219" t="str">
         <v>In Use</v>
@@ -10017,10 +10017,10 @@
         <v>ILOG</v>
       </c>
       <c r="H219" t="str">
-        <v>2022-06-08</v>
+        <v>2018-11-28</v>
       </c>
       <c r="I219" t="str">
-        <v>MISC VENDOR</v>
+        <v>Cybernetic Genesis Private Limited</v>
       </c>
       <c r="J219" t="str">
         <v>Owned</v>
@@ -10029,7 +10029,7 @@
         <v>HO</v>
       </c>
       <c r="L219" t="str">
-        <v>PROJECTION SCREEN</v>
+        <v>PROJECTOR MOUNT KIT</v>
       </c>
       <c r="M219" t="str">
         <v>IT SUPPORT</v>
@@ -10043,25 +10043,25 @@
         <v>Accessories</v>
       </c>
       <c r="B220" t="str">
-        <v>Comrack</v>
+        <v>Generic</v>
       </c>
       <c r="C220" t="str">
-        <v>Comrack</v>
+        <v>PMKIT002</v>
       </c>
       <c r="D220" t="str">
-        <v>CRKHO004</v>
+        <v>PMKIT002</v>
       </c>
       <c r="E220" t="str">
-        <v>ACC-000015</v>
+        <v>ACC-000012</v>
       </c>
       <c r="F220" t="str">
-        <v>Spare</v>
+        <v>In Use</v>
       </c>
       <c r="G220" t="str">
         <v>ILOG</v>
       </c>
       <c r="H220" t="str">
-        <v>2018-11-24</v>
+        <v>2018-11-28</v>
       </c>
       <c r="I220" t="str">
         <v>Cybernetic Genesis Private Limited</v>
@@ -10073,7 +10073,7 @@
         <v>HO</v>
       </c>
       <c r="L220" t="str">
-        <v>EQUIPMENT SHELF RACK</v>
+        <v>PROJECTOR MOUNT KIT</v>
       </c>
       <c r="M220" t="str">
         <v>IT SUPPORT</v>
@@ -10084,31 +10084,31 @@
     </row>
     <row r="221">
       <c r="A221" t="str">
-        <v>Barcode Printer</v>
+        <v>Accessories</v>
       </c>
       <c r="B221" t="str">
-        <v>Postek</v>
+        <v>Generic</v>
       </c>
       <c r="C221" t="str">
-        <v>C-168/200S</v>
+        <v>PSCR001</v>
       </c>
       <c r="D221" t="str">
-        <v>C0716A0225</v>
+        <v>PSCR001</v>
       </c>
       <c r="E221" t="str">
-        <v>BAR-0001</v>
+        <v>ACC-000013</v>
       </c>
       <c r="F221" t="str">
-        <v>Spare</v>
+        <v>In Use</v>
       </c>
       <c r="G221" t="str">
         <v>ILOG</v>
       </c>
       <c r="H221" t="str">
-        <v>2016-04-27</v>
+        <v>2018-11-28</v>
       </c>
       <c r="I221" t="str">
-        <v>Best barcode Systems Private Limited</v>
+        <v>Cybernetic Genesis Private Limited</v>
       </c>
       <c r="J221" t="str">
         <v>Owned</v>
@@ -10117,7 +10117,7 @@
         <v>HO</v>
       </c>
       <c r="L221" t="str">
-        <v>Barcode Printer</v>
+        <v>PROJECTION SCREEN</v>
       </c>
       <c r="M221" t="str">
         <v>IT SUPPORT</v>
@@ -10128,31 +10128,31 @@
     </row>
     <row r="222">
       <c r="A222" t="str">
-        <v>Barcode Printer</v>
+        <v>Accessories</v>
       </c>
       <c r="B222" t="str">
-        <v>Postek</v>
+        <v>Generic</v>
       </c>
       <c r="C222" t="str">
-        <v>C-168/200S</v>
+        <v>PSCR002</v>
       </c>
       <c r="D222" t="str">
-        <v>C0716A0429</v>
+        <v>PSCR002</v>
       </c>
       <c r="E222" t="str">
-        <v>BAR-0002</v>
+        <v>ACC-000014</v>
       </c>
       <c r="F222" t="str">
-        <v>Spare</v>
+        <v>In Use</v>
       </c>
       <c r="G222" t="str">
         <v>ILOG</v>
       </c>
       <c r="H222" t="str">
-        <v>2016-04-27</v>
+        <v>2022-06-08</v>
       </c>
       <c r="I222" t="str">
-        <v>Best barcode Systems Private Limited</v>
+        <v>MISC VENDOR</v>
       </c>
       <c r="J222" t="str">
         <v>Owned</v>
@@ -10161,7 +10161,7 @@
         <v>HO</v>
       </c>
       <c r="L222" t="str">
-        <v>Barcode Printer</v>
+        <v>PROJECTION SCREEN</v>
       </c>
       <c r="M222" t="str">
         <v>IT SUPPORT</v>
@@ -10172,19 +10172,19 @@
     </row>
     <row r="223">
       <c r="A223" t="str">
-        <v>Barcode Printer</v>
+        <v>Accessories</v>
       </c>
       <c r="B223" t="str">
-        <v>Postek</v>
+        <v>Comrack</v>
       </c>
       <c r="C223" t="str">
-        <v>C-168/200S</v>
+        <v>Comrack</v>
       </c>
       <c r="D223" t="str">
-        <v>C0716A0144</v>
+        <v>CRKHO004</v>
       </c>
       <c r="E223" t="str">
-        <v>BAR-0003</v>
+        <v>ACC-000015</v>
       </c>
       <c r="F223" t="str">
         <v>Spare</v>
@@ -10193,19 +10193,19 @@
         <v>ILOG</v>
       </c>
       <c r="H223" t="str">
-        <v>2016-05-31</v>
+        <v>2018-11-24</v>
       </c>
       <c r="I223" t="str">
-        <v>Best barcode Systems Private Limited</v>
+        <v>Cybernetic Genesis Private Limited</v>
       </c>
       <c r="J223" t="str">
         <v>Owned</v>
       </c>
       <c r="K223" t="str">
-        <v>AHM-AWL</v>
+        <v>HO</v>
       </c>
       <c r="L223" t="str">
-        <v>Barcode Printer</v>
+        <v>EQUIPMENT SHELF RACK</v>
       </c>
       <c r="M223" t="str">
         <v>IT SUPPORT</v>
@@ -10225,19 +10225,19 @@
         <v>C-168/200S</v>
       </c>
       <c r="D224" t="str">
-        <v>C0716A0143</v>
+        <v>C0716A0225</v>
       </c>
       <c r="E224" t="str">
-        <v>BAR-0004</v>
+        <v>BAR-0001</v>
       </c>
       <c r="F224" t="str">
-        <v>In Use</v>
+        <v>Spare</v>
       </c>
       <c r="G224" t="str">
         <v>ILOG</v>
       </c>
       <c r="H224" t="str">
-        <v>2016-05-31</v>
+        <v>2016-04-27</v>
       </c>
       <c r="I224" t="str">
         <v>Best barcode Systems Private Limited</v>
@@ -10246,7 +10246,7 @@
         <v>Owned</v>
       </c>
       <c r="K224" t="str">
-        <v>AHM-AWL</v>
+        <v>HO</v>
       </c>
       <c r="L224" t="str">
         <v>Barcode Printer</v>
@@ -10266,31 +10266,31 @@
         <v>Postek</v>
       </c>
       <c r="C225" t="str">
-        <v>C168/200+</v>
+        <v>C-168/200S</v>
       </c>
       <c r="D225" t="str">
-        <v>C3517K0002</v>
+        <v>C0716A0429</v>
       </c>
       <c r="E225" t="str">
-        <v>BAR-0005</v>
+        <v>BAR-0002</v>
       </c>
       <c r="F225" t="str">
-        <v>In Use</v>
+        <v>Spare</v>
       </c>
       <c r="G225" t="str">
         <v>ILOG</v>
       </c>
       <c r="H225" t="str">
-        <v>2020-04-01</v>
+        <v>2016-04-27</v>
       </c>
       <c r="I225" t="str">
-        <v>Trackfins India</v>
+        <v>Best barcode Systems Private Limited</v>
       </c>
       <c r="J225" t="str">
         <v>Owned</v>
       </c>
       <c r="K225" t="str">
-        <v>BLR-AWL</v>
+        <v>HO</v>
       </c>
       <c r="L225" t="str">
         <v>Barcode Printer</v>
@@ -10313,19 +10313,19 @@
         <v>C-168/200S</v>
       </c>
       <c r="D226" t="str">
-        <v>C0176A0174</v>
+        <v>C0716A0144</v>
       </c>
       <c r="E226" t="str">
-        <v>BAR-0006</v>
+        <v>BAR-0003</v>
       </c>
       <c r="F226" t="str">
-        <v>In Use</v>
+        <v>Spare</v>
       </c>
       <c r="G226" t="str">
         <v>ILOG</v>
       </c>
       <c r="H226" t="str">
-        <v>2016-04-27</v>
+        <v>2016-05-31</v>
       </c>
       <c r="I226" t="str">
         <v>Best barcode Systems Private Limited</v>
@@ -10334,7 +10334,7 @@
         <v>Owned</v>
       </c>
       <c r="K226" t="str">
-        <v>BLR-AWL</v>
+        <v>AHM-AWL</v>
       </c>
       <c r="L226" t="str">
         <v>Barcode Printer</v>
@@ -10357,10 +10357,10 @@
         <v>C-168/200S</v>
       </c>
       <c r="D227" t="str">
-        <v>C0716A0173</v>
+        <v>C0716A0143</v>
       </c>
       <c r="E227" t="str">
-        <v>BAR-0007</v>
+        <v>BAR-0004</v>
       </c>
       <c r="F227" t="str">
         <v>In Use</v>
@@ -10369,7 +10369,7 @@
         <v>ILOG</v>
       </c>
       <c r="H227" t="str">
-        <v>2016-04-27</v>
+        <v>2016-05-31</v>
       </c>
       <c r="I227" t="str">
         <v>Best barcode Systems Private Limited</v>
@@ -10378,7 +10378,7 @@
         <v>Owned</v>
       </c>
       <c r="K227" t="str">
-        <v>BLR-AWL</v>
+        <v>AHM-AWL</v>
       </c>
       <c r="L227" t="str">
         <v>Barcode Printer</v>
@@ -10401,10 +10401,10 @@
         <v>C168/200+</v>
       </c>
       <c r="D228" t="str">
-        <v>C3517K0063</v>
+        <v>C3517K0002</v>
       </c>
       <c r="E228" t="str">
-        <v>BAR-0008</v>
+        <v>BAR-0005</v>
       </c>
       <c r="F228" t="str">
         <v>In Use</v>
@@ -10413,7 +10413,7 @@
         <v>ILOG</v>
       </c>
       <c r="H228" t="str">
-        <v>2021-10-30</v>
+        <v>2020-04-01</v>
       </c>
       <c r="I228" t="str">
         <v>Trackfins India</v>
@@ -10422,7 +10422,7 @@
         <v>Owned</v>
       </c>
       <c r="K228" t="str">
-        <v>BIR-AWL</v>
+        <v>BLR-AWL</v>
       </c>
       <c r="L228" t="str">
         <v>Barcode Printer</v>
@@ -10442,13 +10442,13 @@
         <v>Postek</v>
       </c>
       <c r="C229" t="str">
-        <v>C168/200S</v>
+        <v>C-168/200S</v>
       </c>
       <c r="D229" t="str">
-        <v>C0716A0129</v>
+        <v>C0176A0174</v>
       </c>
       <c r="E229" t="str">
-        <v>BAR-0009</v>
+        <v>BAR-0006</v>
       </c>
       <c r="F229" t="str">
         <v>In Use</v>
@@ -10457,7 +10457,7 @@
         <v>ILOG</v>
       </c>
       <c r="H229" t="str">
-        <v>2016-03-01</v>
+        <v>2016-04-27</v>
       </c>
       <c r="I229" t="str">
         <v>Best barcode Systems Private Limited</v>
@@ -10466,7 +10466,7 @@
         <v>Owned</v>
       </c>
       <c r="K229" t="str">
-        <v>BIR-AWL</v>
+        <v>BLR-AWL</v>
       </c>
       <c r="L229" t="str">
         <v>Barcode Printer</v>
@@ -10489,19 +10489,19 @@
         <v>C-168/200S</v>
       </c>
       <c r="D230" t="str">
-        <v>C0716A0203</v>
+        <v>C0716A0173</v>
       </c>
       <c r="E230" t="str">
-        <v>BAR-0010</v>
+        <v>BAR-0007</v>
       </c>
       <c r="F230" t="str">
-        <v>Spare</v>
+        <v>In Use</v>
       </c>
       <c r="G230" t="str">
         <v>ILOG</v>
       </c>
       <c r="H230" t="str">
-        <v>2016-05-19</v>
+        <v>2016-04-27</v>
       </c>
       <c r="I230" t="str">
         <v>Best barcode Systems Private Limited</v>
@@ -10510,7 +10510,7 @@
         <v>Owned</v>
       </c>
       <c r="K230" t="str">
-        <v>MAA-AWL</v>
+        <v>BLR-AWL</v>
       </c>
       <c r="L230" t="str">
         <v>Barcode Printer</v>
@@ -10530,13 +10530,13 @@
         <v>Postek</v>
       </c>
       <c r="C231" t="str">
-        <v>C-168/200S</v>
+        <v>C168/200+</v>
       </c>
       <c r="D231" t="str">
-        <v>C0716A0204</v>
+        <v>C3517K0063</v>
       </c>
       <c r="E231" t="str">
-        <v>BAR-0011</v>
+        <v>BAR-0008</v>
       </c>
       <c r="F231" t="str">
         <v>In Use</v>
@@ -10545,16 +10545,16 @@
         <v>ILOG</v>
       </c>
       <c r="H231" t="str">
-        <v>2016-05-19</v>
+        <v>2021-10-30</v>
       </c>
       <c r="I231" t="str">
-        <v>Best barcode Systems Private Limited</v>
+        <v>Trackfins India</v>
       </c>
       <c r="J231" t="str">
         <v>Owned</v>
       </c>
       <c r="K231" t="str">
-        <v>MAA-AWL</v>
+        <v>BIR-AWL</v>
       </c>
       <c r="L231" t="str">
         <v>Barcode Printer</v>
@@ -10574,13 +10574,13 @@
         <v>Postek</v>
       </c>
       <c r="C232" t="str">
-        <v>C-168 with Lan Cable</v>
+        <v>C168/200S</v>
       </c>
       <c r="D232" t="str">
-        <v>C3517G0211</v>
+        <v>C0716A0129</v>
       </c>
       <c r="E232" t="str">
-        <v>BAR-0012</v>
+        <v>BAR-0009</v>
       </c>
       <c r="F232" t="str">
         <v>In Use</v>
@@ -10589,7 +10589,7 @@
         <v>ILOG</v>
       </c>
       <c r="H232" t="str">
-        <v>2016-04-27</v>
+        <v>2016-03-01</v>
       </c>
       <c r="I232" t="str">
         <v>Best barcode Systems Private Limited</v>
@@ -10598,7 +10598,7 @@
         <v>Owned</v>
       </c>
       <c r="K232" t="str">
-        <v>MAA-AWL</v>
+        <v>BIR-AWL</v>
       </c>
       <c r="L232" t="str">
         <v>Barcode Printer</v>
@@ -10618,22 +10618,22 @@
         <v>Postek</v>
       </c>
       <c r="C233" t="str">
-        <v>C168/200S</v>
+        <v>C-168/200S</v>
       </c>
       <c r="D233" t="str">
-        <v>C0716A0293</v>
+        <v>C0716A0203</v>
       </c>
       <c r="E233" t="str">
-        <v>BAR-0013</v>
+        <v>BAR-0010</v>
       </c>
       <c r="F233" t="str">
-        <v>Faulty</v>
+        <v>Spare</v>
       </c>
       <c r="G233" t="str">
         <v>ILOG</v>
       </c>
       <c r="H233" t="str">
-        <v>2016-03-01</v>
+        <v>2016-05-19</v>
       </c>
       <c r="I233" t="str">
         <v>Best barcode Systems Private Limited</v>
@@ -10642,7 +10642,7 @@
         <v>Owned</v>
       </c>
       <c r="K233" t="str">
-        <v>DEL-AWL</v>
+        <v>MAA-AWL</v>
       </c>
       <c r="L233" t="str">
         <v>Barcode Printer</v>
@@ -10665,10 +10665,10 @@
         <v>C-168/200S</v>
       </c>
       <c r="D234" t="str">
-        <v>C0716A0313</v>
+        <v>C0716A0204</v>
       </c>
       <c r="E234" t="str">
-        <v>BAR-0014</v>
+        <v>BAR-0011</v>
       </c>
       <c r="F234" t="str">
         <v>In Use</v>
@@ -10677,7 +10677,7 @@
         <v>ILOG</v>
       </c>
       <c r="H234" t="str">
-        <v>2016-03-01</v>
+        <v>2016-05-19</v>
       </c>
       <c r="I234" t="str">
         <v>Best barcode Systems Private Limited</v>
@@ -10686,7 +10686,7 @@
         <v>Owned</v>
       </c>
       <c r="K234" t="str">
-        <v>DEL-AWL</v>
+        <v>MAA-AWL</v>
       </c>
       <c r="L234" t="str">
         <v>Barcode Printer</v>
@@ -10706,31 +10706,31 @@
         <v>Postek</v>
       </c>
       <c r="C235" t="str">
-        <v>C-168</v>
+        <v>C-168 with Lan Cable</v>
       </c>
       <c r="D235" t="str">
-        <v>C3517G0117</v>
+        <v>C3517G0211</v>
       </c>
       <c r="E235" t="str">
-        <v>BAR-0015</v>
+        <v>BAR-0012</v>
       </c>
       <c r="F235" t="str">
-        <v>Faulty</v>
+        <v>In Use</v>
       </c>
       <c r="G235" t="str">
-        <v>AWL</v>
+        <v>ILOG</v>
       </c>
       <c r="H235" t="str">
-        <v>2018-01-09</v>
+        <v>2016-04-27</v>
       </c>
       <c r="I235" t="str">
-        <v>Trackfins India</v>
+        <v>Best barcode Systems Private Limited</v>
       </c>
       <c r="J235" t="str">
         <v>Owned</v>
       </c>
       <c r="K235" t="str">
-        <v>HO</v>
+        <v>MAA-AWL</v>
       </c>
       <c r="L235" t="str">
         <v>Barcode Printer</v>
@@ -10753,28 +10753,28 @@
         <v>C168/200S</v>
       </c>
       <c r="D236" t="str">
-        <v>C0716A0253</v>
+        <v>C0716A0293</v>
       </c>
       <c r="E236" t="str">
-        <v>BAR-0016</v>
+        <v>BAR-0013</v>
       </c>
       <c r="F236" t="str">
         <v>Faulty</v>
       </c>
       <c r="G236" t="str">
-        <v>AWL</v>
+        <v>ILOG</v>
       </c>
       <c r="H236" t="str">
-        <v>2016-04-27</v>
+        <v>2016-03-01</v>
       </c>
       <c r="I236" t="str">
-        <v>Trackfins India</v>
+        <v>Best barcode Systems Private Limited</v>
       </c>
       <c r="J236" t="str">
         <v>Owned</v>
       </c>
       <c r="K236" t="str">
-        <v>HO</v>
+        <v>DEL-AWL</v>
       </c>
       <c r="L236" t="str">
         <v>Barcode Printer</v>
@@ -10794,31 +10794,31 @@
         <v>Postek</v>
       </c>
       <c r="C237" t="str">
-        <v>C168/200+</v>
+        <v>C-168/200S</v>
       </c>
       <c r="D237" t="str">
-        <v>C4921J0025</v>
+        <v>C0716A0313</v>
       </c>
       <c r="E237" t="str">
-        <v>BAR-0017</v>
+        <v>BAR-0014</v>
       </c>
       <c r="F237" t="str">
-        <v>Spare</v>
+        <v>In Use</v>
       </c>
       <c r="G237" t="str">
         <v>ILOG</v>
       </c>
       <c r="H237" t="str">
-        <v>2021-11-23</v>
+        <v>2016-03-01</v>
       </c>
       <c r="I237" t="str">
-        <v>Trackfins India</v>
+        <v>Best barcode Systems Private Limited</v>
       </c>
       <c r="J237" t="str">
         <v>Owned</v>
       </c>
       <c r="K237" t="str">
-        <v>HO</v>
+        <v>DEL-AWL</v>
       </c>
       <c r="L237" t="str">
         <v>Barcode Printer</v>
@@ -10838,22 +10838,22 @@
         <v>Postek</v>
       </c>
       <c r="C238" t="str">
-        <v>C-168/200S</v>
+        <v>C-168</v>
       </c>
       <c r="D238" t="str">
-        <v>C0716A0354</v>
+        <v>C3517G0117</v>
       </c>
       <c r="E238" t="str">
-        <v>BAR-0018</v>
+        <v>BAR-0015</v>
       </c>
       <c r="F238" t="str">
-        <v>Spare</v>
+        <v>Faulty</v>
       </c>
       <c r="G238" t="str">
-        <v>ILOG</v>
+        <v>AWL</v>
       </c>
       <c r="H238" t="str">
-        <v>2017-11-28</v>
+        <v>2018-01-09</v>
       </c>
       <c r="I238" t="str">
         <v>Trackfins India</v>
@@ -10879,25 +10879,25 @@
         <v>Barcode Printer</v>
       </c>
       <c r="B239" t="str">
-        <v>TSC</v>
+        <v>Postek</v>
       </c>
       <c r="C239" t="str">
-        <v>TE210</v>
+        <v>C168/200S</v>
       </c>
       <c r="D239" t="str">
-        <v>TEA21180706</v>
+        <v>C0716A0253</v>
       </c>
       <c r="E239" t="str">
-        <v>BAR-0019</v>
+        <v>BAR-0016</v>
       </c>
       <c r="F239" t="str">
-        <v>In Use</v>
+        <v>Faulty</v>
       </c>
       <c r="G239" t="str">
-        <v>ILOG</v>
+        <v>AWL</v>
       </c>
       <c r="H239" t="str">
-        <v>2021-11-11</v>
+        <v>2016-04-27</v>
       </c>
       <c r="I239" t="str">
         <v>Trackfins India</v>
@@ -10923,25 +10923,25 @@
         <v>Barcode Printer</v>
       </c>
       <c r="B240" t="str">
-        <v>TSC</v>
+        <v>Postek</v>
       </c>
       <c r="C240" t="str">
-        <v>TSC 20RB</v>
+        <v>C168/200+</v>
       </c>
       <c r="D240" t="str">
-        <v>T085P21450067</v>
+        <v>C4921J0025</v>
       </c>
       <c r="E240" t="str">
-        <v>BAR-0020</v>
+        <v>BAR-0017</v>
       </c>
       <c r="F240" t="str">
-        <v>In Use</v>
+        <v>Spare</v>
       </c>
       <c r="G240" t="str">
         <v>ILOG</v>
       </c>
       <c r="H240" t="str">
-        <v>2022-08-05</v>
+        <v>2021-11-23</v>
       </c>
       <c r="I240" t="str">
         <v>Trackfins India</v>
@@ -10967,25 +10967,25 @@
         <v>Barcode Printer</v>
       </c>
       <c r="B241" t="str">
-        <v>TSC</v>
+        <v>Postek</v>
       </c>
       <c r="C241" t="str">
-        <v>TSC TTP 244 PRO</v>
+        <v>C-168/200S</v>
       </c>
       <c r="D241" t="str">
-        <v>24P21471731</v>
+        <v>C0716A0354</v>
       </c>
       <c r="E241" t="str">
-        <v>BAR-0021</v>
+        <v>BAR-0018</v>
       </c>
       <c r="F241" t="str">
-        <v>In Use</v>
+        <v>Spare</v>
       </c>
       <c r="G241" t="str">
         <v>ILOG</v>
       </c>
       <c r="H241" t="str">
-        <v>2022-03-04</v>
+        <v>2017-11-28</v>
       </c>
       <c r="I241" t="str">
         <v>Trackfins India</v>
@@ -10994,7 +10994,7 @@
         <v>Owned</v>
       </c>
       <c r="K241" t="str">
-        <v>GGN1-AWL</v>
+        <v>HO</v>
       </c>
       <c r="L241" t="str">
         <v>Barcode Printer</v>
@@ -11014,13 +11014,13 @@
         <v>TSC</v>
       </c>
       <c r="C242" t="str">
-        <v>TSC TTP 244 PRO</v>
+        <v>TE210</v>
       </c>
       <c r="D242" t="str">
-        <v>24P21471712</v>
+        <v>TEA21180706</v>
       </c>
       <c r="E242" t="str">
-        <v>BAR-0022</v>
+        <v>BAR-0019</v>
       </c>
       <c r="F242" t="str">
         <v>In Use</v>
@@ -11029,7 +11029,7 @@
         <v>ILOG</v>
       </c>
       <c r="H242" t="str">
-        <v>2022-03-04</v>
+        <v>2021-11-11</v>
       </c>
       <c r="I242" t="str">
         <v>Trackfins India</v>
@@ -11038,7 +11038,7 @@
         <v>Owned</v>
       </c>
       <c r="K242" t="str">
-        <v>GGN1-AWL</v>
+        <v>HO</v>
       </c>
       <c r="L242" t="str">
         <v>Barcode Printer</v>
@@ -11058,13 +11058,13 @@
         <v>TSC</v>
       </c>
       <c r="C243" t="str">
-        <v>TSC TTP 244 PRO</v>
+        <v>TSC 20RB</v>
       </c>
       <c r="D243" t="str">
-        <v>24P21471739</v>
+        <v>T085P21450067</v>
       </c>
       <c r="E243" t="str">
-        <v>BAR-0023</v>
+        <v>BAR-0020</v>
       </c>
       <c r="F243" t="str">
         <v>In Use</v>
@@ -11073,7 +11073,7 @@
         <v>ILOG</v>
       </c>
       <c r="H243" t="str">
-        <v>2022-03-04</v>
+        <v>2022-08-05</v>
       </c>
       <c r="I243" t="str">
         <v>Trackfins India</v>
@@ -11099,34 +11099,34 @@
         <v>Barcode Printer</v>
       </c>
       <c r="B244" t="str">
-        <v>Postek</v>
+        <v>TSC</v>
       </c>
       <c r="C244" t="str">
-        <v>C-168/200S</v>
+        <v>TSC TTP 244 PRO</v>
       </c>
       <c r="D244" t="str">
-        <v>C01716A0261</v>
+        <v>24P21471731</v>
       </c>
       <c r="E244" t="str">
-        <v>BAR-0024</v>
+        <v>BAR-0021</v>
       </c>
       <c r="F244" t="str">
-        <v>Spare</v>
+        <v>In Use</v>
       </c>
       <c r="G244" t="str">
         <v>ILOG</v>
       </c>
       <c r="H244" t="str">
-        <v>2016-05-31</v>
+        <v>2022-03-04</v>
       </c>
       <c r="I244" t="str">
-        <v>Best barcode Systems Private Limited</v>
+        <v>Trackfins India</v>
       </c>
       <c r="J244" t="str">
         <v>Owned</v>
       </c>
       <c r="K244" t="str">
-        <v>HYD-AWL</v>
+        <v>GGN1-AWL</v>
       </c>
       <c r="L244" t="str">
         <v>Barcode Printer</v>
@@ -11143,16 +11143,16 @@
         <v>Barcode Printer</v>
       </c>
       <c r="B245" t="str">
-        <v>Postek</v>
+        <v>TSC</v>
       </c>
       <c r="C245" t="str">
-        <v>C168/200+</v>
+        <v>TSC TTP 244 PRO</v>
       </c>
       <c r="D245" t="str">
-        <v>C4921J0003</v>
+        <v>24P21471712</v>
       </c>
       <c r="E245" t="str">
-        <v>BAR-0025</v>
+        <v>BAR-0022</v>
       </c>
       <c r="F245" t="str">
         <v>In Use</v>
@@ -11161,7 +11161,7 @@
         <v>ILOG</v>
       </c>
       <c r="H245" t="str">
-        <v>2021-11-23</v>
+        <v>2022-03-04</v>
       </c>
       <c r="I245" t="str">
         <v>Trackfins India</v>
@@ -11170,7 +11170,7 @@
         <v>Owned</v>
       </c>
       <c r="K245" t="str">
-        <v>HYD-AWL</v>
+        <v>GGN1-AWL</v>
       </c>
       <c r="L245" t="str">
         <v>Barcode Printer</v>
@@ -11187,16 +11187,16 @@
         <v>Barcode Printer</v>
       </c>
       <c r="B246" t="str">
-        <v>Postek</v>
+        <v>TSC</v>
       </c>
       <c r="C246" t="str">
-        <v>C168/200+</v>
+        <v>TSC TTP 244 PRO</v>
       </c>
       <c r="D246" t="str">
-        <v>C4921J0004</v>
+        <v>24P21471739</v>
       </c>
       <c r="E246" t="str">
-        <v>BAR-0026</v>
+        <v>BAR-0023</v>
       </c>
       <c r="F246" t="str">
         <v>In Use</v>
@@ -11205,7 +11205,7 @@
         <v>ILOG</v>
       </c>
       <c r="H246" t="str">
-        <v>2021-11-23</v>
+        <v>2022-03-04</v>
       </c>
       <c r="I246" t="str">
         <v>Trackfins India</v>
@@ -11214,7 +11214,7 @@
         <v>Owned</v>
       </c>
       <c r="K246" t="str">
-        <v>HYD-AWL</v>
+        <v>HO</v>
       </c>
       <c r="L246" t="str">
         <v>Barcode Printer</v>
@@ -11237,13 +11237,13 @@
         <v>C-168/200S</v>
       </c>
       <c r="D247" t="str">
-        <v>C01716A0262</v>
+        <v>C01716A0261</v>
       </c>
       <c r="E247" t="str">
-        <v>BAR-0027</v>
+        <v>BAR-0024</v>
       </c>
       <c r="F247" t="str">
-        <v>In Use</v>
+        <v>Spare</v>
       </c>
       <c r="G247" t="str">
         <v>ILOG</v>
@@ -11278,13 +11278,13 @@
         <v>Postek</v>
       </c>
       <c r="C248" t="str">
-        <v>C-168/200S</v>
+        <v>C168/200+</v>
       </c>
       <c r="D248" t="str">
-        <v>C0716A0249</v>
+        <v>C4921J0003</v>
       </c>
       <c r="E248" t="str">
-        <v>BAR-0028</v>
+        <v>BAR-0025</v>
       </c>
       <c r="F248" t="str">
         <v>In Use</v>
@@ -11293,16 +11293,16 @@
         <v>ILOG</v>
       </c>
       <c r="H248" t="str">
-        <v>2016-04-28</v>
+        <v>2021-11-23</v>
       </c>
       <c r="I248" t="str">
-        <v>Best barcode Systems Private Limited</v>
+        <v>Trackfins India</v>
       </c>
       <c r="J248" t="str">
         <v>Owned</v>
       </c>
       <c r="K248" t="str">
-        <v>CCU-AWL</v>
+        <v>HYD-AWL</v>
       </c>
       <c r="L248" t="str">
         <v>Barcode Printer</v>
@@ -11322,13 +11322,13 @@
         <v>Postek</v>
       </c>
       <c r="C249" t="str">
-        <v>C-168/200S</v>
+        <v>C168/200+</v>
       </c>
       <c r="D249" t="str">
-        <v>C0716A0250</v>
+        <v>C4921J0004</v>
       </c>
       <c r="E249" t="str">
-        <v>BAR-0029</v>
+        <v>BAR-0026</v>
       </c>
       <c r="F249" t="str">
         <v>In Use</v>
@@ -11337,16 +11337,16 @@
         <v>ILOG</v>
       </c>
       <c r="H249" t="str">
-        <v>2016-04-28</v>
+        <v>2021-11-23</v>
       </c>
       <c r="I249" t="str">
-        <v>Best barcode Systems Private Limited</v>
+        <v>Trackfins India</v>
       </c>
       <c r="J249" t="str">
         <v>Owned</v>
       </c>
       <c r="K249" t="str">
-        <v>CCU-AWL</v>
+        <v>HYD-AWL</v>
       </c>
       <c r="L249" t="str">
         <v>Barcode Printer</v>
@@ -11369,10 +11369,10 @@
         <v>C-168/200S</v>
       </c>
       <c r="D250" t="str">
-        <v>C0716A0103</v>
+        <v>C01716A0262</v>
       </c>
       <c r="E250" t="str">
-        <v>BAR-0030</v>
+        <v>BAR-0027</v>
       </c>
       <c r="F250" t="str">
         <v>In Use</v>
@@ -11381,7 +11381,7 @@
         <v>ILOG</v>
       </c>
       <c r="H250" t="str">
-        <v>2016-05-21</v>
+        <v>2016-05-31</v>
       </c>
       <c r="I250" t="str">
         <v>Best barcode Systems Private Limited</v>
@@ -11390,7 +11390,7 @@
         <v>Owned</v>
       </c>
       <c r="K250" t="str">
-        <v>LKO-AWL</v>
+        <v>HYD-AWL</v>
       </c>
       <c r="L250" t="str">
         <v>Barcode Printer</v>
@@ -11413,10 +11413,10 @@
         <v>C-168/200S</v>
       </c>
       <c r="D251" t="str">
-        <v>C0716A0185</v>
+        <v>C0716A0249</v>
       </c>
       <c r="E251" t="str">
-        <v>BAR-0031</v>
+        <v>BAR-0028</v>
       </c>
       <c r="F251" t="str">
         <v>In Use</v>
@@ -11425,7 +11425,7 @@
         <v>ILOG</v>
       </c>
       <c r="H251" t="str">
-        <v>2016-05-19</v>
+        <v>2016-04-28</v>
       </c>
       <c r="I251" t="str">
         <v>Best barcode Systems Private Limited</v>
@@ -11434,7 +11434,7 @@
         <v>Owned</v>
       </c>
       <c r="K251" t="str">
-        <v>LKO-AWL</v>
+        <v>CCU-AWL</v>
       </c>
       <c r="L251" t="str">
         <v>Barcode Printer</v>
@@ -11454,31 +11454,31 @@
         <v>Postek</v>
       </c>
       <c r="C252" t="str">
-        <v>C168/200DPI</v>
+        <v>C-168/200S</v>
       </c>
       <c r="D252" t="str">
-        <v>C3517K0081</v>
+        <v>C0716A0250</v>
       </c>
       <c r="E252" t="str">
-        <v>BAR-0032</v>
+        <v>BAR-0029</v>
       </c>
       <c r="F252" t="str">
-        <v>Spare</v>
+        <v>In Use</v>
       </c>
       <c r="G252" t="str">
         <v>ILOG</v>
       </c>
       <c r="H252" t="str">
-        <v>2018-06-26</v>
+        <v>2016-04-28</v>
       </c>
       <c r="I252" t="str">
-        <v>Trackfins India</v>
+        <v>Best barcode Systems Private Limited</v>
       </c>
       <c r="J252" t="str">
         <v>Owned</v>
       </c>
       <c r="K252" t="str">
-        <v>BOM-AWL</v>
+        <v>CCU-AWL</v>
       </c>
       <c r="L252" t="str">
         <v>Barcode Printer</v>
@@ -11498,13 +11498,13 @@
         <v>Postek</v>
       </c>
       <c r="C253" t="str">
-        <v>C168/200DPI</v>
+        <v>C-168/200S</v>
       </c>
       <c r="D253" t="str">
-        <v>C3517K0082</v>
+        <v>C0716A0103</v>
       </c>
       <c r="E253" t="str">
-        <v>BAR-0033</v>
+        <v>BAR-0030</v>
       </c>
       <c r="F253" t="str">
         <v>In Use</v>
@@ -11513,16 +11513,16 @@
         <v>ILOG</v>
       </c>
       <c r="H253" t="str">
-        <v>2018-06-26</v>
+        <v>2016-05-21</v>
       </c>
       <c r="I253" t="str">
-        <v>Trackfins India</v>
+        <v>Best barcode Systems Private Limited</v>
       </c>
       <c r="J253" t="str">
         <v>Owned</v>
       </c>
       <c r="K253" t="str">
-        <v>BOM-AWL</v>
+        <v>LKO-AWL</v>
       </c>
       <c r="L253" t="str">
         <v>Barcode Printer</v>
@@ -11545,10 +11545,10 @@
         <v>C-168/200S</v>
       </c>
       <c r="D254" t="str">
-        <v>C0716A0226</v>
+        <v>C0716A0185</v>
       </c>
       <c r="E254" t="str">
-        <v>BAR-0034</v>
+        <v>BAR-0031</v>
       </c>
       <c r="F254" t="str">
         <v>In Use</v>
@@ -11557,7 +11557,7 @@
         <v>ILOG</v>
       </c>
       <c r="H254" t="str">
-        <v>2016-04-27</v>
+        <v>2016-05-19</v>
       </c>
       <c r="I254" t="str">
         <v>Best barcode Systems Private Limited</v>
@@ -11566,7 +11566,7 @@
         <v>Owned</v>
       </c>
       <c r="K254" t="str">
-        <v>PNQ-AWL</v>
+        <v>LKO-AWL</v>
       </c>
       <c r="L254" t="str">
         <v>Barcode Printer</v>
@@ -11586,22 +11586,22 @@
         <v>Postek</v>
       </c>
       <c r="C255" t="str">
-        <v>C-168/200+</v>
+        <v>C168/200DPI</v>
       </c>
       <c r="D255" t="str">
-        <v>C3517G0084</v>
+        <v>C3517K0081</v>
       </c>
       <c r="E255" t="str">
-        <v>BAR-0035</v>
+        <v>BAR-0032</v>
       </c>
       <c r="F255" t="str">
-        <v>In Use</v>
+        <v>Spare</v>
       </c>
       <c r="G255" t="str">
         <v>ILOG</v>
       </c>
       <c r="H255" t="str">
-        <v>2017-12-12</v>
+        <v>2018-06-26</v>
       </c>
       <c r="I255" t="str">
         <v>Trackfins India</v>
@@ -11610,7 +11610,7 @@
         <v>Owned</v>
       </c>
       <c r="K255" t="str">
-        <v>AHM-AWL</v>
+        <v>BOM-AWL</v>
       </c>
       <c r="L255" t="str">
         <v>Barcode Printer</v>
@@ -11624,19 +11624,19 @@
     </row>
     <row r="256">
       <c r="A256" t="str">
-        <v>Attendance Machine</v>
+        <v>Barcode Printer</v>
       </c>
       <c r="B256" t="str">
-        <v>Matrix</v>
+        <v>Postek</v>
       </c>
       <c r="C256" t="str">
-        <v>COSEC DOOR V3</v>
+        <v>C168/200DPI</v>
       </c>
       <c r="D256" t="str">
-        <v>10009329</v>
+        <v>C3517K0082</v>
       </c>
       <c r="E256" t="str">
-        <v>ATT-000001</v>
+        <v>BAR-0033</v>
       </c>
       <c r="F256" t="str">
         <v>In Use</v>
@@ -11645,19 +11645,19 @@
         <v>ILOG</v>
       </c>
       <c r="H256" t="str">
-        <v>2018-12-19</v>
+        <v>2018-06-26</v>
       </c>
       <c r="I256" t="str">
-        <v>Cybernetic Genesis Private Limited</v>
+        <v>Trackfins India</v>
       </c>
       <c r="J256" t="str">
         <v>Owned</v>
       </c>
       <c r="K256" t="str">
-        <v>HO</v>
+        <v>BOM-AWL</v>
       </c>
       <c r="L256" t="str">
-        <v>Biometric - Attendance Machine</v>
+        <v>Barcode Printer</v>
       </c>
       <c r="M256" t="str">
         <v>IT SUPPORT</v>
@@ -11668,19 +11668,19 @@
     </row>
     <row r="257">
       <c r="A257" t="str">
-        <v>Attendance Machine</v>
+        <v>Barcode Printer</v>
       </c>
       <c r="B257" t="str">
-        <v>Matrix</v>
+        <v>Postek</v>
       </c>
       <c r="C257" t="str">
-        <v>COSEC DOOR V3</v>
+        <v>C-168/200S</v>
       </c>
       <c r="D257" t="str">
-        <v>10008975</v>
+        <v>C0716A0226</v>
       </c>
       <c r="E257" t="str">
-        <v>ATT-000002</v>
+        <v>BAR-0034</v>
       </c>
       <c r="F257" t="str">
         <v>In Use</v>
@@ -11689,19 +11689,19 @@
         <v>ILOG</v>
       </c>
       <c r="H257" t="str">
-        <v>2018-12-19</v>
+        <v>2016-04-27</v>
       </c>
       <c r="I257" t="str">
-        <v>Cybernetic Genesis Private Limited</v>
+        <v>Best barcode Systems Private Limited</v>
       </c>
       <c r="J257" t="str">
         <v>Owned</v>
       </c>
       <c r="K257" t="str">
-        <v>AHM-AWL</v>
+        <v>PNQ-AWL</v>
       </c>
       <c r="L257" t="str">
-        <v>Biometric - Attendance Machine</v>
+        <v>Barcode Printer</v>
       </c>
       <c r="M257" t="str">
         <v>IT SUPPORT</v>
@@ -11712,19 +11712,19 @@
     </row>
     <row r="258">
       <c r="A258" t="str">
-        <v>Attendance Machine</v>
+        <v>Barcode Printer</v>
       </c>
       <c r="B258" t="str">
-        <v>Matrix</v>
+        <v>Postek</v>
       </c>
       <c r="C258" t="str">
-        <v>COSEC DOOR V3</v>
+        <v>C-168/200+</v>
       </c>
       <c r="D258" t="str">
-        <v>10008967</v>
+        <v>C3517G0084</v>
       </c>
       <c r="E258" t="str">
-        <v>ATT-000003</v>
+        <v>BAR-0035</v>
       </c>
       <c r="F258" t="str">
         <v>In Use</v>
@@ -11733,19 +11733,19 @@
         <v>ILOG</v>
       </c>
       <c r="H258" t="str">
-        <v>2018-12-19</v>
+        <v>2017-12-12</v>
       </c>
       <c r="I258" t="str">
-        <v>Cybernetic Genesis Private Limited</v>
+        <v>Trackfins India</v>
       </c>
       <c r="J258" t="str">
         <v>Owned</v>
       </c>
       <c r="K258" t="str">
-        <v>BLR-AWL</v>
+        <v>AHM-AWL</v>
       </c>
       <c r="L258" t="str">
-        <v>Biometric - Attendance Machine</v>
+        <v>Barcode Printer</v>
       </c>
       <c r="M258" t="str">
         <v>IT SUPPORT</v>
@@ -11765,10 +11765,10 @@
         <v>COSEC DOOR V3</v>
       </c>
       <c r="D259" t="str">
-        <v>10008947</v>
+        <v>10009329</v>
       </c>
       <c r="E259" t="str">
-        <v>ATT-000004</v>
+        <v>ATT-000001</v>
       </c>
       <c r="F259" t="str">
         <v>In Use</v>
@@ -11786,7 +11786,7 @@
         <v>Owned</v>
       </c>
       <c r="K259" t="str">
-        <v>BIR-AWL</v>
+        <v>HO</v>
       </c>
       <c r="L259" t="str">
         <v>Biometric - Attendance Machine</v>
@@ -11809,10 +11809,10 @@
         <v>COSEC DOOR V3</v>
       </c>
       <c r="D260" t="str">
-        <v>10008944</v>
+        <v>10008975</v>
       </c>
       <c r="E260" t="str">
-        <v>ATT-000005</v>
+        <v>ATT-000002</v>
       </c>
       <c r="F260" t="str">
         <v>In Use</v>
@@ -11830,7 +11830,7 @@
         <v>Owned</v>
       </c>
       <c r="K260" t="str">
-        <v>MAA-AWL</v>
+        <v>AHM-AWL</v>
       </c>
       <c r="L260" t="str">
         <v>Biometric - Attendance Machine</v>
@@ -11853,10 +11853,10 @@
         <v>COSEC DOOR V3</v>
       </c>
       <c r="D261" t="str">
-        <v>10008948</v>
+        <v>10008967</v>
       </c>
       <c r="E261" t="str">
-        <v>ATT-000006</v>
+        <v>ATT-000003</v>
       </c>
       <c r="F261" t="str">
         <v>In Use</v>
@@ -11874,7 +11874,7 @@
         <v>Owned</v>
       </c>
       <c r="K261" t="str">
-        <v>DEL-AWL</v>
+        <v>BLR-AWL</v>
       </c>
       <c r="L261" t="str">
         <v>Biometric - Attendance Machine</v>
@@ -11897,13 +11897,13 @@
         <v>COSEC DOOR V3</v>
       </c>
       <c r="D262" t="str">
-        <v>10008953</v>
+        <v>10008947</v>
       </c>
       <c r="E262" t="str">
-        <v>ATT-000007</v>
+        <v>ATT-000004</v>
       </c>
       <c r="F262" t="str">
-        <v>Spare</v>
+        <v>In Use</v>
       </c>
       <c r="G262" t="str">
         <v>ILOG</v>
@@ -11918,7 +11918,7 @@
         <v>Owned</v>
       </c>
       <c r="K262" t="str">
-        <v>HO</v>
+        <v>BIR-AWL</v>
       </c>
       <c r="L262" t="str">
         <v>Biometric - Attendance Machine</v>
@@ -11935,34 +11935,34 @@
         <v>Attendance Machine</v>
       </c>
       <c r="B263" t="str">
-        <v>Vantage</v>
+        <v>Matrix</v>
       </c>
       <c r="C263" t="str">
-        <v>VA-600-CTA</v>
+        <v>COSEC DOOR V3</v>
       </c>
       <c r="D263" t="str">
-        <v>201406000308</v>
+        <v>10008944</v>
       </c>
       <c r="E263" t="str">
-        <v>ATT-000008</v>
+        <v>ATT-000005</v>
       </c>
       <c r="F263" t="str">
-        <v>Spare</v>
+        <v>In Use</v>
       </c>
       <c r="G263" t="str">
         <v>ILOG</v>
       </c>
       <c r="H263" t="str">
-        <v>2015-08-27</v>
+        <v>2018-12-19</v>
       </c>
       <c r="I263" t="str">
-        <v>JBV Security Solution</v>
+        <v>Cybernetic Genesis Private Limited</v>
       </c>
       <c r="J263" t="str">
         <v>Owned</v>
       </c>
       <c r="K263" t="str">
-        <v>HO</v>
+        <v>MAA-AWL</v>
       </c>
       <c r="L263" t="str">
         <v>Biometric - Attendance Machine</v>
@@ -11979,34 +11979,34 @@
         <v>Attendance Machine</v>
       </c>
       <c r="B264" t="str">
-        <v>Vantage</v>
+        <v>Matrix</v>
       </c>
       <c r="C264" t="str">
-        <v>VA-800-CTA</v>
+        <v>COSEC DOOR V3</v>
       </c>
       <c r="D264" t="str">
-        <v>201406000411</v>
+        <v>10008948</v>
       </c>
       <c r="E264" t="str">
-        <v>ATT-000009</v>
+        <v>ATT-000006</v>
       </c>
       <c r="F264" t="str">
-        <v>Spare</v>
+        <v>In Use</v>
       </c>
       <c r="G264" t="str">
-        <v>AWL</v>
+        <v>ILOG</v>
       </c>
       <c r="H264" t="str">
-        <v>2020-04-01</v>
+        <v>2018-12-19</v>
       </c>
       <c r="I264" t="str">
-        <v>MISC VENDOR</v>
+        <v>Cybernetic Genesis Private Limited</v>
       </c>
       <c r="J264" t="str">
         <v>Owned</v>
       </c>
       <c r="K264" t="str">
-        <v>HO</v>
+        <v>DEL-AWL</v>
       </c>
       <c r="L264" t="str">
         <v>Biometric - Attendance Machine</v>
@@ -12029,13 +12029,13 @@
         <v>COSEC DOOR V3</v>
       </c>
       <c r="D265" t="str">
-        <v>10009388</v>
+        <v>10008953</v>
       </c>
       <c r="E265" t="str">
-        <v>ATT-000010</v>
+        <v>ATT-000007</v>
       </c>
       <c r="F265" t="str">
-        <v>In Use</v>
+        <v>Spare</v>
       </c>
       <c r="G265" t="str">
         <v>ILOG</v>
@@ -12067,34 +12067,34 @@
         <v>Attendance Machine</v>
       </c>
       <c r="B266" t="str">
-        <v>Matrix</v>
+        <v>Vantage</v>
       </c>
       <c r="C266" t="str">
-        <v>COSEC DOOR V3</v>
+        <v>VA-600-CTA</v>
       </c>
       <c r="D266" t="str">
-        <v>10008950</v>
+        <v>201406000308</v>
       </c>
       <c r="E266" t="str">
-        <v>ATT-000011</v>
+        <v>ATT-000008</v>
       </c>
       <c r="F266" t="str">
-        <v>In Use</v>
+        <v>Spare</v>
       </c>
       <c r="G266" t="str">
         <v>ILOG</v>
       </c>
       <c r="H266" t="str">
-        <v>2018-12-19</v>
+        <v>2015-08-27</v>
       </c>
       <c r="I266" t="str">
-        <v>Cybernetic Genesis Private Limited</v>
+        <v>JBV Security Solution</v>
       </c>
       <c r="J266" t="str">
         <v>Owned</v>
       </c>
       <c r="K266" t="str">
-        <v>GGN1-AWL</v>
+        <v>HO</v>
       </c>
       <c r="L266" t="str">
         <v>Biometric - Attendance Machine</v>
@@ -12114,31 +12114,31 @@
         <v>Vantage</v>
       </c>
       <c r="C267" t="str">
-        <v>VA-600-CTA</v>
+        <v>VA-800-CTA</v>
       </c>
       <c r="D267" t="str">
-        <v>201406000280</v>
+        <v>201406000411</v>
       </c>
       <c r="E267" t="str">
-        <v>ATT-000012</v>
+        <v>ATT-000009</v>
       </c>
       <c r="F267" t="str">
         <v>Spare</v>
       </c>
       <c r="G267" t="str">
-        <v>ILOG</v>
+        <v>AWL</v>
       </c>
       <c r="H267" t="str">
-        <v>2015-08-27</v>
+        <v>2020-04-01</v>
       </c>
       <c r="I267" t="str">
-        <v>JBV Security Solution</v>
+        <v>MISC VENDOR</v>
       </c>
       <c r="J267" t="str">
         <v>Owned</v>
       </c>
       <c r="K267" t="str">
-        <v>GGN2-AWL</v>
+        <v>HO</v>
       </c>
       <c r="L267" t="str">
         <v>Biometric - Attendance Machine</v>
@@ -12161,10 +12161,10 @@
         <v>COSEC DOOR V3</v>
       </c>
       <c r="D268" t="str">
-        <v>10008951</v>
+        <v>10009388</v>
       </c>
       <c r="E268" t="str">
-        <v>ATT-000013</v>
+        <v>ATT-000010</v>
       </c>
       <c r="F268" t="str">
         <v>In Use</v>
@@ -12182,7 +12182,7 @@
         <v>Owned</v>
       </c>
       <c r="K268" t="str">
-        <v>GGN2-AWL</v>
+        <v>HO</v>
       </c>
       <c r="L268" t="str">
         <v>Biometric - Attendance Machine</v>
@@ -12205,10 +12205,10 @@
         <v>COSEC DOOR V3</v>
       </c>
       <c r="D269" t="str">
-        <v>10009821</v>
+        <v>10008950</v>
       </c>
       <c r="E269" t="str">
-        <v>ATT-000014</v>
+        <v>ATT-000011</v>
       </c>
       <c r="F269" t="str">
         <v>In Use</v>
@@ -12217,7 +12217,7 @@
         <v>ILOG</v>
       </c>
       <c r="H269" t="str">
-        <v>2019-01-14</v>
+        <v>2018-12-19</v>
       </c>
       <c r="I269" t="str">
         <v>Cybernetic Genesis Private Limited</v>
@@ -12226,7 +12226,7 @@
         <v>Owned</v>
       </c>
       <c r="K269" t="str">
-        <v>HYD-AWL</v>
+        <v>GGN1-AWL</v>
       </c>
       <c r="L269" t="str">
         <v>Biometric - Attendance Machine</v>
@@ -12243,34 +12243,34 @@
         <v>Attendance Machine</v>
       </c>
       <c r="B270" t="str">
-        <v>Matrix</v>
+        <v>Vantage</v>
       </c>
       <c r="C270" t="str">
-        <v>COSEC DOOR V3</v>
+        <v>VA-600-CTA</v>
       </c>
       <c r="D270" t="str">
-        <v>10008960</v>
+        <v>201406000280</v>
       </c>
       <c r="E270" t="str">
-        <v>ATT-000015</v>
+        <v>ATT-000012</v>
       </c>
       <c r="F270" t="str">
-        <v>In Use</v>
+        <v>Spare</v>
       </c>
       <c r="G270" t="str">
         <v>ILOG</v>
       </c>
       <c r="H270" t="str">
-        <v>2018-12-19</v>
+        <v>2015-08-27</v>
       </c>
       <c r="I270" t="str">
-        <v>Cybernetic Genesis Private Limited</v>
+        <v>JBV Security Solution</v>
       </c>
       <c r="J270" t="str">
         <v>Owned</v>
       </c>
       <c r="K270" t="str">
-        <v>CCU-AWL</v>
+        <v>GGN2-AWL</v>
       </c>
       <c r="L270" t="str">
         <v>Biometric - Attendance Machine</v>
@@ -12293,10 +12293,10 @@
         <v>COSEC DOOR V3</v>
       </c>
       <c r="D271" t="str">
-        <v>10008954</v>
+        <v>10008951</v>
       </c>
       <c r="E271" t="str">
-        <v>ATT-000016</v>
+        <v>ATT-000013</v>
       </c>
       <c r="F271" t="str">
         <v>In Use</v>
@@ -12314,7 +12314,7 @@
         <v>Owned</v>
       </c>
       <c r="K271" t="str">
-        <v>LKO-AWL</v>
+        <v>GGN2-AWL</v>
       </c>
       <c r="L271" t="str">
         <v>Biometric - Attendance Machine</v>
@@ -12337,10 +12337,10 @@
         <v>COSEC DOOR V3</v>
       </c>
       <c r="D272" t="str">
-        <v>10008968</v>
+        <v>10009821</v>
       </c>
       <c r="E272" t="str">
-        <v>ATT-000017</v>
+        <v>ATT-000014</v>
       </c>
       <c r="F272" t="str">
         <v>In Use</v>
@@ -12349,7 +12349,7 @@
         <v>ILOG</v>
       </c>
       <c r="H272" t="str">
-        <v>2018-12-19</v>
+        <v>2019-01-14</v>
       </c>
       <c r="I272" t="str">
         <v>Cybernetic Genesis Private Limited</v>
@@ -12358,7 +12358,7 @@
         <v>Owned</v>
       </c>
       <c r="K272" t="str">
-        <v>BOM-AWL</v>
+        <v>HYD-AWL</v>
       </c>
       <c r="L272" t="str">
         <v>Biometric - Attendance Machine</v>
@@ -12381,16 +12381,16 @@
         <v>COSEC DOOR V3</v>
       </c>
       <c r="D273" t="str">
-        <v>10009333</v>
+        <v>10008960</v>
       </c>
       <c r="E273" t="str">
-        <v>ATT-000018</v>
+        <v>ATT-000015</v>
       </c>
       <c r="F273" t="str">
         <v>In Use</v>
       </c>
       <c r="G273" t="str">
-        <v>AWL</v>
+        <v>ILOG</v>
       </c>
       <c r="H273" t="str">
         <v>2018-12-19</v>
@@ -12402,7 +12402,7 @@
         <v>Owned</v>
       </c>
       <c r="K273" t="str">
-        <v>PNQ-AWL</v>
+        <v>CCU-AWL</v>
       </c>
       <c r="L273" t="str">
         <v>Biometric - Attendance Machine</v>
@@ -12416,19 +12416,19 @@
     </row>
     <row r="274">
       <c r="A274" t="str">
-        <v>Amplifier</v>
+        <v>Attendance Machine</v>
       </c>
       <c r="B274" t="str">
-        <v>Bose</v>
+        <v>Matrix</v>
       </c>
       <c r="C274" t="str">
-        <v>3448714410</v>
+        <v>COSEC DOOR V3</v>
       </c>
       <c r="D274" t="str">
-        <v>056392H81700045AE</v>
+        <v>10008954</v>
       </c>
       <c r="E274" t="str">
-        <v>AMP-000001</v>
+        <v>ATT-000016</v>
       </c>
       <c r="F274" t="str">
         <v>In Use</v>
@@ -12437,19 +12437,19 @@
         <v>ILOG</v>
       </c>
       <c r="H274" t="str">
-        <v>2018-10-26</v>
+        <v>2018-12-19</v>
       </c>
       <c r="I274" t="str">
-        <v>Total tech Solutions</v>
+        <v>Cybernetic Genesis Private Limited</v>
       </c>
       <c r="J274" t="str">
         <v>Owned</v>
       </c>
       <c r="K274" t="str">
-        <v>HO</v>
+        <v>LKO-AWL</v>
       </c>
       <c r="L274" t="str">
-        <v>Bose Amplifier</v>
+        <v>Biometric - Attendance Machine</v>
       </c>
       <c r="M274" t="str">
         <v>IT SUPPORT</v>
@@ -12460,19 +12460,19 @@
     </row>
     <row r="275">
       <c r="A275" t="str">
-        <v>Amplifier</v>
+        <v>Attendance Machine</v>
       </c>
       <c r="B275" t="str">
-        <v>Bose</v>
+        <v>Matrix</v>
       </c>
       <c r="C275" t="str">
-        <v>3448714410</v>
+        <v>COSEC DOOR V3</v>
       </c>
       <c r="D275" t="str">
-        <v>059881F81220034AE</v>
+        <v>10008968</v>
       </c>
       <c r="E275" t="str">
-        <v>AMP-000002</v>
+        <v>ATT-000017</v>
       </c>
       <c r="F275" t="str">
         <v>In Use</v>
@@ -12481,19 +12481,19 @@
         <v>ILOG</v>
       </c>
       <c r="H275" t="str">
-        <v>2018-10-26</v>
+        <v>2018-12-19</v>
       </c>
       <c r="I275" t="str">
-        <v>Total tech Solutions</v>
+        <v>Cybernetic Genesis Private Limited</v>
       </c>
       <c r="J275" t="str">
         <v>Owned</v>
       </c>
       <c r="K275" t="str">
-        <v>HO</v>
+        <v>BOM-AWL</v>
       </c>
       <c r="L275" t="str">
-        <v>Bose Amplifier</v>
+        <v>Biometric - Attendance Machine</v>
       </c>
       <c r="M275" t="str">
         <v>IT SUPPORT</v>
@@ -12502,9 +12502,141 @@
         <v>IT 6771</v>
       </c>
     </row>
+    <row r="276">
+      <c r="A276" t="str">
+        <v>Attendance Machine</v>
+      </c>
+      <c r="B276" t="str">
+        <v>Matrix</v>
+      </c>
+      <c r="C276" t="str">
+        <v>COSEC DOOR V3</v>
+      </c>
+      <c r="D276" t="str">
+        <v>10009333</v>
+      </c>
+      <c r="E276" t="str">
+        <v>ATT-000018</v>
+      </c>
+      <c r="F276" t="str">
+        <v>In Use</v>
+      </c>
+      <c r="G276" t="str">
+        <v>AWL</v>
+      </c>
+      <c r="H276" t="str">
+        <v>2018-12-19</v>
+      </c>
+      <c r="I276" t="str">
+        <v>Cybernetic Genesis Private Limited</v>
+      </c>
+      <c r="J276" t="str">
+        <v>Owned</v>
+      </c>
+      <c r="K276" t="str">
+        <v>PNQ-AWL</v>
+      </c>
+      <c r="L276" t="str">
+        <v>Biometric - Attendance Machine</v>
+      </c>
+      <c r="M276" t="str">
+        <v>IT SUPPORT</v>
+      </c>
+      <c r="N276" t="str">
+        <v>IT 6771</v>
+      </c>
+    </row>
+    <row r="277">
+      <c r="A277" t="str">
+        <v>Amplifier</v>
+      </c>
+      <c r="B277" t="str">
+        <v>Bose</v>
+      </c>
+      <c r="C277" t="str">
+        <v>3448714410</v>
+      </c>
+      <c r="D277" t="str">
+        <v>056392H81700045AE</v>
+      </c>
+      <c r="E277" t="str">
+        <v>AMP-000001</v>
+      </c>
+      <c r="F277" t="str">
+        <v>In Use</v>
+      </c>
+      <c r="G277" t="str">
+        <v>ILOG</v>
+      </c>
+      <c r="H277" t="str">
+        <v>2018-10-26</v>
+      </c>
+      <c r="I277" t="str">
+        <v>Total tech Solutions</v>
+      </c>
+      <c r="J277" t="str">
+        <v>Owned</v>
+      </c>
+      <c r="K277" t="str">
+        <v>HO</v>
+      </c>
+      <c r="L277" t="str">
+        <v>Bose Amplifier</v>
+      </c>
+      <c r="M277" t="str">
+        <v>IT SUPPORT</v>
+      </c>
+      <c r="N277" t="str">
+        <v>IT 6771</v>
+      </c>
+    </row>
+    <row r="278">
+      <c r="A278" t="str">
+        <v>Amplifier</v>
+      </c>
+      <c r="B278" t="str">
+        <v>Bose</v>
+      </c>
+      <c r="C278" t="str">
+        <v>3448714410</v>
+      </c>
+      <c r="D278" t="str">
+        <v>059881F81220034AE</v>
+      </c>
+      <c r="E278" t="str">
+        <v>AMP-000002</v>
+      </c>
+      <c r="F278" t="str">
+        <v>In Use</v>
+      </c>
+      <c r="G278" t="str">
+        <v>ILOG</v>
+      </c>
+      <c r="H278" t="str">
+        <v>2018-10-26</v>
+      </c>
+      <c r="I278" t="str">
+        <v>Total tech Solutions</v>
+      </c>
+      <c r="J278" t="str">
+        <v>Owned</v>
+      </c>
+      <c r="K278" t="str">
+        <v>HO</v>
+      </c>
+      <c r="L278" t="str">
+        <v>Bose Amplifier</v>
+      </c>
+      <c r="M278" t="str">
+        <v>IT SUPPORT</v>
+      </c>
+      <c r="N278" t="str">
+        <v>IT 6771</v>
+      </c>
+    </row>
   </sheetData>
   <ignoredErrors>
-    <ignoredError numberStoredAsText="1" sqref="A1:N275"/>
+    <ignoredError numberStoredAsText="1" sqref="A1:N278"/>
   </ignoredErrors>
 </worksheet>
 </file>
</xml_diff>